<commit_message>
update for distinct sampling of the cell concentraion
</commit_message>
<xml_diff>
--- a/input_files/fed_batch_data2.xlsx
+++ b/input_files/fed_batch_data2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galileo/development/Reserch/UMN_Research/CCDPA_git/CCDPApy/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904AEC90-7B2B-BF42-8693-DE90F3F08C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E083DE5A-FAD0-7C42-B20E-9393EA6FA86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" activeTab="2" xr2:uid="{C7583198-B141-1C4B-B50F-A9FA90CFEBEA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{C7583198-B141-1C4B-B50F-A9FA90CFEBEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Measured Data" sheetId="1" r:id="rId1"/>
@@ -1021,11 +1021,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE2EEBC-76CD-9641-BDBB-B5D8CDAAE100}">
   <dimension ref="A1:BN150"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BP15" sqref="BP15"/>
+      <selection pane="bottomRight" activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3284,9 +3284,7 @@
       <c r="N16" s="14">
         <v>0.24155578300921182</v>
       </c>
-      <c r="O16" s="14">
-        <v>0</v>
-      </c>
+      <c r="O16" s="14"/>
       <c r="P16" s="32">
         <v>0</v>
       </c>
@@ -3716,9 +3714,7 @@
       <c r="N19" s="14">
         <v>1.5747241725175525</v>
       </c>
-      <c r="O19" s="14">
-        <v>2.947953065515585</v>
-      </c>
+      <c r="O19" s="14"/>
       <c r="P19" s="32">
         <v>0</v>
       </c>
@@ -4292,9 +4288,7 @@
       <c r="N23" s="14">
         <v>17.659352142110759</v>
       </c>
-      <c r="O23" s="14">
-        <v>46.224693064601453</v>
-      </c>
+      <c r="O23" s="14"/>
       <c r="P23" s="32">
         <v>0.28967406250000005</v>
       </c>
@@ -4580,9 +4574,7 @@
       <c r="N25" s="14">
         <v>22.010582010582009</v>
       </c>
-      <c r="O25" s="14">
-        <v>105.27343257531042</v>
-      </c>
+      <c r="O25" s="14"/>
       <c r="P25" s="32">
         <v>0.29504359760156251</v>
       </c>
@@ -20216,7 +20208,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20915,7 +20907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E44892B-DFB0-9045-8086-D16FEC8C5180}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>